<commit_message>
201022 add download and compare result fuction
</commit_message>
<xml_diff>
--- a/比對結果.xlsx
+++ b/比對結果.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="新細明體"/>
       <family val="2"/>
@@ -32,6 +32,9 @@
     <font>
       <b val="1"/>
       <sz val="14"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -54,12 +57,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -72,12 +78,12 @@
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
-      <col>3</col>
+      <col>1</col>
       <colOff>0</colOff>
       <row>3</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1524000" cy="857250"/>
+    <ext cx="952500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr descr="Picture" id="1" name="Image 1"/>
@@ -97,12 +103,12 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>4</col>
+      <col>3</col>
       <colOff>0</colOff>
       <row>3</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1524000" cy="857250"/>
+    <ext cx="952500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr descr="Picture" id="2" name="Image 2"/>
@@ -122,12 +128,12 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>3</col>
+      <col>1</col>
       <colOff>0</colOff>
       <row>4</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1524000" cy="857250"/>
+    <ext cx="952500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr descr="Picture" id="3" name="Image 3"/>
@@ -147,12 +153,12 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>4</col>
+      <col>3</col>
       <colOff>0</colOff>
       <row>4</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1524000" cy="857250"/>
+    <ext cx="952500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr descr="Picture" id="4" name="Image 4"/>
@@ -464,7 +470,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,10 +478,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="40"/>
-    <col customWidth="1" max="2" min="2" width="40"/>
-    <col customWidth="1" max="4" min="4" width="25"/>
-    <col customWidth="1" max="5" min="5" width="25"/>
+    <col customWidth="1" max="1" min="1" width="50"/>
+    <col customWidth="1" max="2" min="2" width="20"/>
+    <col customWidth="1" max="3" min="3" width="50"/>
+    <col customWidth="1" max="4" min="4" width="20"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -491,31 +497,43 @@
           <t>工程編號：5B11U0A6</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>日期：2020/10/12</t>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>日期：2020/10/22</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="70" r="4">
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>上傳的相片</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>上傳的相片</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="80" r="4">
       <c r="A4" t="inlineStr">
         <is>
           <t>5B11U0A6_4_001-006.docx_Page001_1.jpg</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>5B11U0A6_4_001-006.docx_Page001_5.jpg</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="70" r="5">
+    <row customHeight="1" ht="80" r="5">
       <c r="A5" t="inlineStr">
         <is>
           <t>5B11U0A6_4_001-006.docx_Page001_2.jpg</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>5B11U0A6_4_001-006.docx_Page001_6.jpg</t>
         </is>
@@ -523,7 +541,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>